<commit_message>
Add menu , modify dishes and ingr database and add ID taker
</commit_message>
<xml_diff>
--- a/Alpha/DB.xlsx
+++ b/Alpha/DB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -43,10 +43,13 @@
     <t>Гречка</t>
   </si>
   <si>
+    <t>Курина грудка</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
-    <t>Капуста с помидором</t>
+    <t>Помидоры с капустой</t>
   </si>
   <si>
     <t>ID:</t>
@@ -68,6 +71,15 @@
   </si>
   <si>
     <t>СумСт (ясли)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма: </t>
+  </si>
+  <si>
+    <t>fhfgh</t>
+  </si>
+  <si>
+    <t>dfglkdf</t>
   </si>
 </sst>
 </file>
@@ -457,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -526,8 +538,19 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
+      </c>
+      <c r="C6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -538,10 +561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,82 +576,348 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>33</v>
-      </c>
-      <c r="C3">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>54</v>
-      </c>
-      <c r="E3">
-        <f>B3*C3/1000</f>
-        <v>1.056</v>
-      </c>
-      <c r="F3">
-        <f>B3*D3/1000</f>
-        <v>1.782</v>
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>0.33</v>
+      </c>
+      <c r="F4">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>55</v>
       </c>
-      <c r="C4">
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+      <c r="E5">
+        <v>2.42</v>
+      </c>
+      <c r="F5">
+        <v>2.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>2.75</v>
+      </c>
+      <c r="F8">
+        <v>3.3660000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>54</v>
-      </c>
-      <c r="E4">
-        <f>B4*C4/1000</f>
-        <v>0.66</v>
-      </c>
-      <c r="F4">
-        <f>B4*D4/1000</f>
-        <v>2.97</v>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>B12*C12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>B12*D12/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>B13*C13/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>B13*D13/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>B14*C14/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>B14*D14/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>B15*C15/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>B15*D15/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f>SUM(E12:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>SUM(F12:F15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>B22*C22/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>B22*D22/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>B23*C23/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>B23*D23/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>33</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f>B24*C24/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>B24*D24/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f>SUM(E22:E24)</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>SUM(F22:F24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start creating fill report system
</commit_message>
<xml_diff>
--- a/Alpha/DB.xlsx
+++ b/Alpha/DB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -31,25 +31,193 @@
     <t>Цена</t>
   </si>
   <si>
-    <t>Помидоры</t>
+    <t>Какао</t>
+  </si>
+  <si>
+    <t>Родзинки</t>
+  </si>
+  <si>
+    <t>Чай</t>
+  </si>
+  <si>
+    <t>Печиво</t>
+  </si>
+  <si>
+    <t>Дріжжі</t>
+  </si>
+  <si>
+    <t>Лавр.лист</t>
+  </si>
+  <si>
+    <t>Ванілін</t>
+  </si>
+  <si>
+    <t>Сіль</t>
+  </si>
+  <si>
+    <t>Молоко згущ.</t>
+  </si>
+  <si>
+    <t>Сметана</t>
+  </si>
+  <si>
+    <t>Макарони</t>
+  </si>
+  <si>
+    <t>Крохмал</t>
+  </si>
+  <si>
+    <t>Огірки сол.</t>
+  </si>
+  <si>
+    <t>Капуста кв.</t>
+  </si>
+  <si>
+    <t>Смородина</t>
+  </si>
+  <si>
+    <t>Зел.Горошок</t>
+  </si>
+  <si>
+    <t>Томат</t>
+  </si>
+  <si>
+    <t>Олія</t>
+  </si>
+  <si>
+    <t>Борошно</t>
+  </si>
+  <si>
+    <t>Рис</t>
+  </si>
+  <si>
+    <t>Горох лущ.</t>
+  </si>
+  <si>
+    <t>Гречана</t>
+  </si>
+  <si>
+    <t>Пшенична</t>
+  </si>
+  <si>
+    <t>Вівсяна</t>
+  </si>
+  <si>
+    <t>Пшоно</t>
+  </si>
+  <si>
+    <t>Манна</t>
+  </si>
+  <si>
+    <t>Ячна</t>
+  </si>
+  <si>
+    <t>Молоко</t>
+  </si>
+  <si>
+    <t>Хліб пшен.</t>
+  </si>
+  <si>
+    <t>Хліб ржан.</t>
+  </si>
+  <si>
+    <t>Масло в.</t>
+  </si>
+  <si>
+    <t>Сир тв.</t>
+  </si>
+  <si>
+    <t>Сир кисл.</t>
+  </si>
+  <si>
+    <t>Філе куряче</t>
+  </si>
+  <si>
+    <t>Кунжут</t>
+  </si>
+  <si>
+    <t>Цукор</t>
+  </si>
+  <si>
+    <t>Щавель</t>
+  </si>
+  <si>
+    <t>Капуста пекінськ.</t>
+  </si>
+  <si>
+    <t>Картопля</t>
+  </si>
+  <si>
+    <t>Морква</t>
+  </si>
+  <si>
+    <t>Буряк</t>
   </si>
   <si>
     <t>Капуста</t>
   </si>
   <si>
-    <t>Салат</t>
-  </si>
-  <si>
-    <t>Гречка</t>
-  </si>
-  <si>
-    <t>Курина грудка</t>
+    <t>Цибуля</t>
+  </si>
+  <si>
+    <t>Огірки свіжі</t>
+  </si>
+  <si>
+    <t>Томати свіжі</t>
+  </si>
+  <si>
+    <t>Малина</t>
+  </si>
+  <si>
+    <t>Слива</t>
+  </si>
+  <si>
+    <t>Перець</t>
+  </si>
+  <si>
+    <t>Баклажани</t>
+  </si>
+  <si>
+    <t>Зелень</t>
+  </si>
+  <si>
+    <t>Кабачки</t>
+  </si>
+  <si>
+    <t>Яйця</t>
+  </si>
+  <si>
+    <t>Вишня</t>
+  </si>
+  <si>
+    <t>Яблука</t>
+  </si>
+  <si>
+    <t>Лимони</t>
+  </si>
+  <si>
+    <t>Повидло</t>
+  </si>
+  <si>
+    <t>Сухофрукти</t>
+  </si>
+  <si>
+    <t>Печінка</t>
+  </si>
+  <si>
+    <t>Яловичина</t>
+  </si>
+  <si>
+    <t>Ментай</t>
+  </si>
+  <si>
+    <t>Сода</t>
   </si>
   <si>
     <t>*</t>
   </si>
   <si>
-    <t>Помидоры с капустой</t>
+    <t>Жопа</t>
   </si>
   <si>
     <t>ID:</t>
@@ -76,10 +244,7 @@
     <t xml:space="preserve">Сумма: </t>
   </si>
   <si>
-    <t>fhfgh</t>
-  </si>
-  <si>
-    <t>dfglkdf</t>
+    <t>Писи</t>
   </si>
 </sst>
 </file>
@@ -469,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -501,7 +666,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="6">
-        <v>33</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -512,7 +677,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -523,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>55</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -534,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -545,14 +710,634 @@
         <v>7</v>
       </c>
       <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>100.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>17.84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>183.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>93.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>14.19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>51.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
+      <c r="C59">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -561,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H29"/>
+  <dimension ref="A2:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +1363,13 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -592,86 +1377,92 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>33</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
       <c r="D4">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="E4">
-        <v>0.33</v>
+        <f>B4*C4/1000</f>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.39600000000000002</v>
+        <f>B4*D4/1000</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="D5">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E5">
-        <v>2.42</v>
+        <f>B5*C5/1000</f>
+        <v>1.444</v>
       </c>
       <c r="F5">
-        <v>2.97</v>
+        <f>B5*D5/1000</f>
+        <v>0.64600000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8">
-        <v>2.75</v>
+        <f>SUM(E4:E5)</f>
+        <v>1.444</v>
       </c>
       <c r="F8">
-        <v>3.3660000000000001</v>
+        <f>SUM(F4:F5)</f>
+        <v>0.64600000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -679,80 +1470,80 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E12">
         <f>B12*C12/1000</f>
-        <v>0</v>
+        <v>1.425</v>
       </c>
       <c r="F12">
         <f>B12*D12/1000</f>
-        <v>0</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E13">
         <f>B13*C13/1000</f>
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="F13">
         <f>B13*D13/1000</f>
-        <v>0</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B14">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <f>B14*C14/1000</f>
@@ -765,159 +1556,49 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B15">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E15">
         <f>B15*C15/1000</f>
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="F15">
         <f>B15*D15/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18">
         <f>SUM(E12:E15)</f>
-        <v>0</v>
+        <v>5.1849999999999996</v>
       </c>
       <c r="F18">
         <f>SUM(F12:F15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <v>33</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f>B22*C22/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <f>B22*D22/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>33</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <f>B23*C23/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <f>B23*D23/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <v>33</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <f>B24*C24/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <f>B24*D24/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E27">
-        <f>SUM(E22:E24)</f>
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <f>SUM(F22:F24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
-        <v>8</v>
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>